<commit_message>
2D_Arrays transform matrix n diagnol_sum
</commit_message>
<xml_diff>
--- a/prep.xlsx
+++ b/prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/stiver/prep/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59E0423-4E74-574A-BA5D-2CD6968FD1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5297CE-5A16-DB4E-B27B-A581A02CA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Video links</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/flipping-an-image/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/matrix-diagonal-sum/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/transpose-matrix/</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -564,9 +570,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -595,6 +609,8 @@
     <hyperlink ref="C10" r:id="rId22" xr:uid="{0256B69D-D788-9145-B562-B9EE8B2AAAA7}"/>
     <hyperlink ref="C11" r:id="rId23" xr:uid="{6C0318BC-F2DF-EE43-B504-E6E32F4314EA}"/>
     <hyperlink ref="C14" r:id="rId24" xr:uid="{FFAC90D5-ED54-F540-9A73-DF1F29E18810}"/>
+    <hyperlink ref="C15" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
+    <hyperlink ref="C16" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sentence pangram or not
</commit_message>
<xml_diff>
--- a/prep.xlsx
+++ b/prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/stiver/prep/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5297CE-5A16-DB4E-B27B-A581A02CA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB514820-D736-CB46-B785-5B2B05FD1AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Video links</t>
   </si>
@@ -122,13 +122,19 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/transpose-matrix/</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/check-if-the-sentence-is-pangram/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,6 +173,22 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,13 +215,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,10 +447,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -450,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -581,6 +609,16 @@
       </c>
       <c r="C16" s="5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -611,6 +649,7 @@
     <hyperlink ref="C14" r:id="rId24" xr:uid="{FFAC90D5-ED54-F540-9A73-DF1F29E18810}"/>
     <hyperlink ref="C15" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
     <hyperlink ref="C16" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
+    <hyperlink ref="C19" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
palindrome number or not
</commit_message>
<xml_diff>
--- a/prep.xlsx
+++ b/prep.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/stiver/prep/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB514820-D736-CB46-B785-5B2B05FD1AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52922461-1F6B-4B45-BE18-2B0455EFF5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Video links</t>
   </si>
@@ -128,6 +129,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/check-if-the-sentence-is-pangram/</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number</t>
   </si>
 </sst>
 </file>
@@ -447,7 +454,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
@@ -619,6 +626,16 @@
     <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C19" s="5" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C22" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -650,7 +667,20 @@
     <hyperlink ref="C15" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
     <hyperlink ref="C16" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
     <hyperlink ref="C19" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
+    <hyperlink ref="C22" r:id="rId28" xr:uid="{7C09D988-960B-DD43-A750-2D576364DCFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C77E028-ADEF-014B-915C-F36A215F19A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cells with Odd Values in a Matrix
</commit_message>
<xml_diff>
--- a/prep.xlsx
+++ b/prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/stiver/prep/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52922461-1F6B-4B45-BE18-2B0455EFF5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532B6231-30F0-0D43-A590-705E0275FF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Video links</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/palindrome-number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/cells-with-odd-values-in-a-matrix/</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="151" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -618,23 +621,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="4" t="s">
+    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="5" t="s">
+    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="5" t="s">
+    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -666,8 +674,9 @@
     <hyperlink ref="C14" r:id="rId24" xr:uid="{FFAC90D5-ED54-F540-9A73-DF1F29E18810}"/>
     <hyperlink ref="C15" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
     <hyperlink ref="C16" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
-    <hyperlink ref="C19" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
-    <hyperlink ref="C22" r:id="rId28" xr:uid="{7C09D988-960B-DD43-A750-2D576364DCFE}"/>
+    <hyperlink ref="C20" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
+    <hyperlink ref="C23" r:id="rId28" xr:uid="{7C09D988-960B-DD43-A750-2D576364DCFE}"/>
+    <hyperlink ref="C17" r:id="rId29" xr:uid="{725C3C7E-A112-EC4A-B5A9-BE4109075DD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1D Arrays - no of good pairs
</commit_message>
<xml_diff>
--- a/prep.xlsx
+++ b/prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/stiver/prep/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532B6231-30F0-0D43-A590-705E0275FF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E468E0-7DD2-B048-8483-928418D16F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Video links</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/cells-with-odd-values-in-a-matrix/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-good-pairs/</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="151" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
@@ -593,10 +596,8 @@
         <v>17</v>
       </c>
       <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="4" t="s">
-        <v>29</v>
+      <c r="C12" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -604,13 +605,13 @@
         <v>18</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -618,31 +619,36 @@
         <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="4" t="s">
+    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="5" t="s">
+    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="4" t="s">
+    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C23" s="5" t="s">
+    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C24" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -671,12 +677,13 @@
     <hyperlink ref="C9" r:id="rId21" xr:uid="{D45CC79A-A70A-1A49-A40E-EE4BA0EA5B17}"/>
     <hyperlink ref="C10" r:id="rId22" xr:uid="{0256B69D-D788-9145-B562-B9EE8B2AAAA7}"/>
     <hyperlink ref="C11" r:id="rId23" xr:uid="{6C0318BC-F2DF-EE43-B504-E6E32F4314EA}"/>
-    <hyperlink ref="C14" r:id="rId24" xr:uid="{FFAC90D5-ED54-F540-9A73-DF1F29E18810}"/>
-    <hyperlink ref="C15" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
-    <hyperlink ref="C16" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
-    <hyperlink ref="C20" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
-    <hyperlink ref="C23" r:id="rId28" xr:uid="{7C09D988-960B-DD43-A750-2D576364DCFE}"/>
-    <hyperlink ref="C17" r:id="rId29" xr:uid="{725C3C7E-A112-EC4A-B5A9-BE4109075DD6}"/>
+    <hyperlink ref="C15" r:id="rId24" xr:uid="{FFAC90D5-ED54-F540-9A73-DF1F29E18810}"/>
+    <hyperlink ref="C16" r:id="rId25" xr:uid="{EA27487E-AFE4-D443-A862-C667FBD09D45}"/>
+    <hyperlink ref="C17" r:id="rId26" xr:uid="{C6DDFDE4-170F-9147-91AD-A18A346FA570}"/>
+    <hyperlink ref="C21" r:id="rId27" xr:uid="{07243129-141E-EF4A-8A99-F4EC11A98E76}"/>
+    <hyperlink ref="C24" r:id="rId28" xr:uid="{7C09D988-960B-DD43-A750-2D576364DCFE}"/>
+    <hyperlink ref="C18" r:id="rId29" xr:uid="{725C3C7E-A112-EC4A-B5A9-BE4109075DD6}"/>
+    <hyperlink ref="C12" r:id="rId30" xr:uid="{291D3DB1-8FBE-D14F-8D4C-BF552EE74175}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>